<commit_message>
Fixed parsing, added HTML option
</commit_message>
<xml_diff>
--- a/src/main/resources/Robinson22Checklist.xlsx
+++ b/src/main/resources/Robinson22Checklist.xlsx
@@ -428,7 +428,7 @@
     <t>Functioning</t>
   </si>
   <si>
-    <t>BEFORE STARTING ENGINE</t>
+    <t>Before Starting Engine</t>
   </si>
   <si>
     <t>Seat Belts</t>
@@ -512,7 +512,7 @@
     <t>Governor Switch</t>
   </si>
   <si>
-    <t>STARTING ENGINE AND RUN-UP</t>
+    <t>Starting Engine and Run Up</t>
   </si>
   <si>
     <t>Throttle Twists For Priming</t>

</xml_diff>